<commit_message>
test cases are changed
</commit_message>
<xml_diff>
--- a/Week_6/non functional testing.xlsx
+++ b/Week_6/non functional testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\QA\Week_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590173EC-9248-4B6C-ACB0-40650418A7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7422B27-AAB4-4642-89E5-614D0BDCC9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E11D5B01-5FAD-41E3-9FCD-543C84D036CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E11D5B01-5FAD-41E3-9FCD-543C84D036CE}"/>
   </bookViews>
   <sheets>
     <sheet name="test environment" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="430">
   <si>
     <t>Hardware</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Risk</t>
   </si>
   <si>
-    <t>HOST_007</t>
-  </si>
-  <si>
     <t>Test Case ID</t>
   </si>
   <si>
@@ -401,9 +398,6 @@
     <t>High (Lack of SSL can lead to security vulnerabilities and loss of user trust)</t>
   </si>
   <si>
-    <t>HOST_004</t>
-  </si>
-  <si>
     <t>SSL Certificates</t>
   </si>
   <si>
@@ -452,9 +446,6 @@
     <t>Medium-High (Inefficient content delivery can lead to slow load times)</t>
   </si>
   <si>
-    <t>HOST_002</t>
-  </si>
-  <si>
     <t>Content Delivery Network (CDN)</t>
   </si>
   <si>
@@ -512,9 +503,6 @@
     <t>High (Slow page load times can lead to poor user experience and increased bounce rates)</t>
   </si>
   <si>
-    <t>HOST_001</t>
-  </si>
-  <si>
     <t>Page Load Time</t>
   </si>
   <si>
@@ -764,75 +752,12 @@
     <t>https://cloud.gatling.io/</t>
   </si>
   <si>
-    <t>Secure Access to Accounts</t>
-  </si>
-  <si>
-    <t>SEC_001</t>
-  </si>
-  <si>
-    <t>High (Unauthorized access can lead to data breaches and user information theft)</t>
-  </si>
-  <si>
-    <t>Verify that user accounts are secure and accessible only by authorized users</t>
-  </si>
-  <si>
-    <t>1. Verify Login Process</t>
-  </si>
-  <si>
-    <t>Enter valid credentials and log in</t>
-  </si>
-  <si>
     <t>User can log in successfully with valid credentials</t>
   </si>
   <si>
-    <t>impossible to test because logout and re-registration functionality is not implemented</t>
-  </si>
-  <si>
-    <t>Verify successful login</t>
-  </si>
-  <si>
-    <t>2. Check Password Policy</t>
-  </si>
-  <si>
-    <t>Attempt to set a weak password</t>
-  </si>
-  <si>
-    <t>System enforces strong password requirements (e.g., minimum length, complexity)</t>
-  </si>
-  <si>
-    <t>Verify password strength requirements</t>
-  </si>
-  <si>
-    <t>3. Test Account Lockout</t>
-  </si>
-  <si>
-    <t>Enter incorrect password multiple times</t>
-  </si>
-  <si>
-    <t>Account is temporarily locked after a certain number of failed login attempts</t>
-  </si>
-  <si>
-    <t>Verify account lockout mechanism</t>
-  </si>
-  <si>
-    <t>4. Verify Logout Functionality</t>
-  </si>
-  <si>
-    <t>Log out from the account</t>
-  </si>
-  <si>
-    <t>User is successfully logged out, and session is terminated</t>
-  </si>
-  <si>
-    <t>Verify user is logged out</t>
-  </si>
-  <si>
     <t>Two-Factor Authentication (2FA)</t>
   </si>
   <si>
-    <t>SEC_002</t>
-  </si>
-  <si>
     <t>High (Lack of 2FA can make accounts vulnerable to unauthorized access)</t>
   </si>
   <si>
@@ -902,9 +827,6 @@
     <t>Encryption of Payment Data</t>
   </si>
   <si>
-    <t>SEC_003</t>
-  </si>
-  <si>
     <t>Very High (Unencrypted payment data can lead to financial fraud and data theft)</t>
   </si>
   <si>
@@ -971,9 +893,6 @@
     <t>Compliance with Safety Standards (PCI DSS)</t>
   </si>
   <si>
-    <t>SEC_004</t>
-  </si>
-  <si>
     <t>Very High (Non-compliance with PCI DSS can result in legal penalties and data breaches)</t>
   </si>
   <si>
@@ -1136,10 +1055,6 @@
     <t>CTAs are prominently displayed and easy to locate</t>
   </si>
   <si>
-    <t>The functionality is implemented partially. Some sections such as the Store are missing. The CTAs that are there have different languages.
-Full testing at this stage is not possible</t>
-  </si>
-  <si>
     <t>2. Test Clickability</t>
   </si>
   <si>
@@ -1299,9 +1214,6 @@
     <t>Spacing between elements is not consistent and visually appealing</t>
   </si>
   <si>
-    <t>On some pages, such as our Store Policies, About Our Store, Support, some elements have different spacing</t>
-  </si>
-  <si>
     <t>4. Validate Margin and Padding</t>
   </si>
   <si>
@@ -1339,6 +1251,148 @@
   </si>
   <si>
     <t>https://prometheusqastage2.wixsite.com/skybot/blank-4</t>
+  </si>
+  <si>
+    <t>NFSEC_001</t>
+  </si>
+  <si>
+    <t>NFSEC_002</t>
+  </si>
+  <si>
+    <t>Authentication Mechanisms</t>
+  </si>
+  <si>
+    <t>Verify that the authentication mechanisms are secure and function correctly</t>
+  </si>
+  <si>
+    <t>High Unauthorized access to user accounts could lead to identity theft, financial loss, and damage to the company's reputation)</t>
+  </si>
+  <si>
+    <t>1. Test Login with Valid Credentials</t>
+  </si>
+  <si>
+    <t>Enter valid username and password</t>
+  </si>
+  <si>
+    <t>Click login</t>
+  </si>
+  <si>
+    <t>2. Test Login with Invalid Credentials</t>
+  </si>
+  <si>
+    <t>Enter invalid username and/or password</t>
+  </si>
+  <si>
+    <t>Attempt to log in</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Login attempt should fail, with an appropriate error message</t>
+  </si>
+  <si>
+    <t>3. Test Brute Force Protection</t>
+  </si>
+  <si>
+    <t>Attempt multiple failed login attempts</t>
+  </si>
+  <si>
+    <t>Check for account lockout or captcha</t>
+  </si>
+  <si>
+    <t>After a specified number of failed attempts, the account should be temporarily locked or require captcha</t>
+  </si>
+  <si>
+    <t>4. Test Password Reset Functionality</t>
+  </si>
+  <si>
+    <t>Request a password reset</t>
+  </si>
+  <si>
+    <t>Verify email or SMS for reset link</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Password reset link should be sent securely, and the user should be able to reset their password</t>
+  </si>
+  <si>
+    <t>NFSEC_003</t>
+  </si>
+  <si>
+    <t>NFSEC_004</t>
+  </si>
+  <si>
+    <t>Protection Against SQL Injection, XSS, CSRF</t>
+  </si>
+  <si>
+    <t>NFSEC_005</t>
+  </si>
+  <si>
+    <t>Ensure that the system is protected against common web vulnerabilities like SQL injection, XSS, and CSRF</t>
+  </si>
+  <si>
+    <t>Critical (These vulnerabilities can lead to unauthorized data access, account takeover, and damage to the website's integrity)</t>
+  </si>
+  <si>
+    <t>1. Test for SQL Injection Vulnerability</t>
+  </si>
+  <si>
+    <t>Input SQL queries into text fields</t>
+  </si>
+  <si>
+    <t>Monitor system behavior</t>
+  </si>
+  <si>
+    <t>The system should properly sanitize inputs and prevent SQL injection attacks. No unintended database queries should be executed</t>
+  </si>
+  <si>
+    <t>2. Test for Cross-Site Scripting (XSS)</t>
+  </si>
+  <si>
+    <t>Input scripts into text fields</t>
+  </si>
+  <si>
+    <t>Check for script execution in the browser</t>
+  </si>
+  <si>
+    <t>The system should sanitize inputs to prevent XSS attacks. No scripts should execute in the browser</t>
+  </si>
+  <si>
+    <t>3. Test for Cross-Site Request Forgery (CSRF)</t>
+  </si>
+  <si>
+    <t>Attempt to perform unauthorized actions via CSRF</t>
+  </si>
+  <si>
+    <t>Observe system response</t>
+  </si>
+  <si>
+    <t>4. Validate Input Validation and Sanitization</t>
+  </si>
+  <si>
+    <t>Input special characters and scripts</t>
+  </si>
+  <si>
+    <t>Observe system behavior</t>
+  </si>
+  <si>
+    <t>All inputs should be validated and sanitized to prevent any injection or scripting vulnerabilities</t>
+  </si>
+  <si>
+    <t>The system should reject unauthorized requests, ensuring that CSRF attacks are not successful</t>
+  </si>
+  <si>
+    <t>NFHOST_001</t>
+  </si>
+  <si>
+    <t>NFHOST_002</t>
+  </si>
+  <si>
+    <t>NFHOST_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The functionality is implemented partially. The CTAs that are there have different languages.
+</t>
+  </si>
+  <si>
+    <t>On some pages, such as About us, Support some elements have different spacing</t>
   </si>
 </sst>
 </file>
@@ -1501,18 +1555,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1524,6 +1566,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2045,10 +2099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EE2585-4408-455E-97CD-87F70D088E16}">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2064,36 +2118,36 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
       <c r="C1" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>136</v>
+        <v>425</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -2102,7 +2156,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -2111,7 +2165,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -2135,20 +2189,20 @@
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A9" s="24" t="s">
-        <v>133</v>
+      <c r="A9" s="27" t="s">
+        <v>130</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>408</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>410</v>
+        <v>129</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>381</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" t="e" vm="1">
@@ -2156,35 +2210,35 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="30">
-      <c r="A10" s="24"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="23"/>
+        <v>127</v>
+      </c>
+      <c r="C10" s="26"/>
       <c r="D10" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="23"/>
+        <v>126</v>
+      </c>
+      <c r="E10" s="26"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:7">
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:7" ht="30">
-      <c r="A12" s="24" t="s">
-        <v>128</v>
+      <c r="A12" s="27" t="s">
+        <v>125</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>409</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>410</v>
+        <v>124</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>381</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" t="e" vm="2">
@@ -2192,59 +2246,59 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="23"/>
+        <v>115</v>
+      </c>
+      <c r="C13" s="26"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="23"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:7">
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="24" t="s">
-        <v>125</v>
+      <c r="A15" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>120</v>
       </c>
       <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="23"/>
+        <v>115</v>
+      </c>
+      <c r="C16" s="26"/>
       <c r="D16" s="13"/>
       <c r="E16" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="D17" s="13"/>
     </row>
     <row r="18" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A18" s="24" t="s">
-        <v>121</v>
+      <c r="A18" s="27" t="s">
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>411</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>410</v>
+        <v>117</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>381</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" t="e" vm="3">
@@ -2252,13 +2306,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A19" s="24"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="23"/>
+        <v>115</v>
+      </c>
+      <c r="C19" s="26"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="23"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1">
@@ -2266,19 +2320,19 @@
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>116</v>
+        <v>426</v>
       </c>
       <c r="D22" s="13"/>
     </row>
@@ -2287,7 +2341,7 @@
         <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D23" s="4"/>
     </row>
@@ -2296,7 +2350,7 @@
         <v>31</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" s="4"/>
     </row>
@@ -2313,92 +2367,88 @@
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:7" ht="22.5" customHeight="1">
-      <c r="A28" s="22" t="s">
-        <v>113</v>
+      <c r="A28" s="28" t="s">
+        <v>111</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>408</v>
-      </c>
-      <c r="E28" s="23" t="s">
         <v>110</v>
       </c>
+      <c r="C28" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>108</v>
+      </c>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A29" s="22"/>
+      <c r="A29" s="28"/>
       <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="23"/>
+        <v>107</v>
+      </c>
+      <c r="C29" s="26"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="23"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="7"/>
       <c r="G29" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="22" t="s">
-        <v>108</v>
+      <c r="A31" s="28" t="s">
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>104</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="23" t="s">
-        <v>105</v>
+      <c r="E31" s="26" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="22"/>
+      <c r="A32" s="28"/>
       <c r="B32" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" s="23"/>
-      <c r="E32" s="23"/>
+        <v>102</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="E32" s="26"/>
     </row>
     <row r="34" spans="1:6" ht="41.25" customHeight="1">
       <c r="A34" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F34" s="7"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="4"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>99</v>
+        <v>427</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30">
@@ -2406,524 +2456,150 @@
         <v>33</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="5"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="30">
       <c r="A40" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>408</v>
-      </c>
-      <c r="E44" t="s">
-        <v>94</v>
-      </c>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="22"/>
-      <c r="B45" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="7"/>
+      <c r="A44" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" ht="30">
+      <c r="A45" s="28"/>
+      <c r="B45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="22"/>
-      <c r="B48" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" t="s">
-        <v>86</v>
-      </c>
-      <c r="C50" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="22"/>
-      <c r="B51" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="7"/>
-    </row>
-    <row r="52" spans="1:6" ht="18.75">
-      <c r="D52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" ht="30">
-      <c r="A53" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D53" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F53" s="7"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:6" ht="18.75">
-      <c r="A55" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B62" t="s">
-        <v>72</v>
-      </c>
-      <c r="C62" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="22"/>
-      <c r="B63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" t="s">
-        <v>69</v>
-      </c>
-      <c r="D63" s="23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="D64" s="23"/>
-    </row>
-    <row r="65" spans="1:4" ht="30">
-      <c r="A65" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D65" s="23"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="22"/>
-      <c r="B66" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" s="23"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="D67" s="23"/>
-    </row>
-    <row r="68" spans="1:4" ht="30">
-      <c r="A68" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="23"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="22"/>
-      <c r="B69" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="18.75">
-      <c r="D70" s="6"/>
-    </row>
-    <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D71" s="5"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="1:4" ht="30">
-      <c r="A73" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D73" s="4"/>
-    </row>
-    <row r="74" spans="1:4" ht="30">
-      <c r="A74" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="22"/>
-      <c r="B79" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="D80" s="23"/>
-    </row>
-    <row r="81" spans="1:7" ht="30">
-      <c r="A81" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D81" s="23"/>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="22"/>
-      <c r="B82" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D82" s="23"/>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="D83" s="23"/>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D84" s="23"/>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" s="22"/>
-      <c r="B85" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="18.75">
-      <c r="A87" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="30">
-      <c r="A89" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="30">
-      <c r="A90" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="18.75">
-      <c r="A92" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D92" s="6"/>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="D93" s="5"/>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D94" s="4"/>
-    </row>
-    <row r="95" spans="1:7" ht="30">
-      <c r="A95" s="22"/>
-      <c r="B95" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D95" s="4"/>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="D96" s="4"/>
-      <c r="G96" s="23"/>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" s="22" t="s">
+      <c r="A47" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D97" s="5"/>
-      <c r="E97" s="4" t="s">
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" ht="30">
+      <c r="A48" s="28"/>
+      <c r="B48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="28"/>
+      <c r="B51" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="18.75">
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="D60" s="4"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="D62" s="5"/>
+    </row>
+    <row r="68" spans="4:6">
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="4:6">
+      <c r="D69" s="4"/>
+    </row>
+    <row r="79" spans="4:6">
+      <c r="E79" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F97" s="7"/>
-      <c r="G97" s="23"/>
-    </row>
-    <row r="98" spans="1:7" ht="30">
-      <c r="A98" s="22"/>
-      <c r="B98" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C98" s="4" t="s">
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="4:6" ht="30">
+      <c r="E80" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E98" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F98" s="7"/>
-      <c r="G98" s="23"/>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="D99" s="4"/>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D100" s="4"/>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="22"/>
-      <c r="B101" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="18.75">
-      <c r="D107" s="6"/>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="D108" s="5"/>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="D109" s="4"/>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="D110" s="4"/>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="D112" s="5"/>
-    </row>
-    <row r="118" spans="4:4">
-      <c r="D118" s="4"/>
-    </row>
-    <row r="119" spans="4:4">
-      <c r="D119" s="4"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="95" spans="7:7">
+      <c r="G95" s="26"/>
+    </row>
+    <row r="96" spans="7:7">
+      <c r="G96" s="26"/>
+    </row>
+    <row r="97" spans="7:7">
+      <c r="G97" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D63:D68"/>
-    <mergeCell ref="D79:D84"/>
-    <mergeCell ref="G96:G98"/>
+  <mergeCells count="21">
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="A12:A13"/>
@@ -2931,33 +2607,19 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C31:C32"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="G95:G97"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E31:E32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D53" r:id="rId1" xr:uid="{BF91C729-B873-42CB-9FAC-B65685F2F628}"/>
-    <hyperlink ref="D44" r:id="rId2" xr:uid="{779F719F-C5D3-40E3-A9B2-D8255895AF46}"/>
-    <hyperlink ref="D28" r:id="rId3" xr:uid="{19DAED4F-73C9-44BC-B04E-CC542485B14B}"/>
-    <hyperlink ref="D18" r:id="rId4" xr:uid="{889E5F36-C5EF-419F-A43B-9C81C224140E}"/>
-    <hyperlink ref="D12" r:id="rId5" xr:uid="{9E49D897-0891-4710-8241-7E58F2A793B1}"/>
-    <hyperlink ref="D9" r:id="rId6" xr:uid="{9194E538-3A69-4A8D-8D6D-7A23A0E96564}"/>
+    <hyperlink ref="D28" r:id="rId1" xr:uid="{19DAED4F-73C9-44BC-B04E-CC542485B14B}"/>
+    <hyperlink ref="D18" r:id="rId2" xr:uid="{889E5F36-C5EF-419F-A43B-9C81C224140E}"/>
+    <hyperlink ref="D12" r:id="rId3" xr:uid="{9E49D897-0891-4710-8241-7E58F2A793B1}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{9194E538-3A69-4A8D-8D6D-7A23A0E96564}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2985,36 +2647,36 @@
     <row r="1" spans="1:7" ht="18.75">
       <c r="B1" s="3"/>
       <c r="C1" s="18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3023,7 +2685,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -3032,7 +2694,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -3052,34 +2714,34 @@
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="28"/>
+      <c r="B10" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="22"/>
-      <c r="B10" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F10" s="15"/>
     </row>
@@ -3087,32 +2749,32 @@
       <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="22" t="s">
-        <v>154</v>
+      <c r="A12" s="28" t="s">
+        <v>150</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="22"/>
+      <c r="A13" s="28"/>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F13" s="7"/>
     </row>
@@ -3120,32 +2782,32 @@
       <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:7" ht="30">
-      <c r="A15" s="22" t="s">
-        <v>159</v>
+      <c r="A15" s="28" t="s">
+        <v>155</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="22"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F16" s="7"/>
     </row>
@@ -3153,32 +2815,32 @@
       <c r="C17" s="13"/>
     </row>
     <row r="18" spans="1:6" ht="30">
-      <c r="A18" s="22" t="s">
-        <v>164</v>
+      <c r="A18" s="28" t="s">
+        <v>160</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="22"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F19" s="7"/>
     </row>
@@ -3187,18 +2849,18 @@
     </row>
     <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30">
@@ -3206,7 +2868,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30">
@@ -3214,7 +2876,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3226,31 +2888,31 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="30">
-      <c r="A29" s="22" t="s">
-        <v>173</v>
+      <c r="A29" s="28" t="s">
+        <v>169</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F29" s="15"/>
     </row>
     <row r="30" spans="1:6" ht="18.75">
-      <c r="A30" s="22"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F30" s="15"/>
     </row>
@@ -3258,29 +2920,29 @@
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="22" t="s">
-        <v>178</v>
+      <c r="A32" s="28" t="s">
+        <v>174</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="22"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F33" s="15"/>
     </row>
@@ -3288,68 +2950,68 @@
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="22" t="s">
-        <v>183</v>
+      <c r="A35" s="28" t="s">
+        <v>179</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="28"/>
+      <c r="B36" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E36" s="26"/>
+    </row>
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="B38" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="22"/>
-      <c r="B36" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E36" s="23"/>
-    </row>
-    <row r="38" spans="1:6" ht="30">
-      <c r="A38" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>186</v>
+      <c r="E38" s="26" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="22"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E39" s="23"/>
+        <v>164</v>
+      </c>
+      <c r="E39" s="26"/>
     </row>
     <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30">
@@ -3357,7 +3019,7 @@
         <v>33</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30">
@@ -3365,7 +3027,7 @@
         <v>31</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18.75">
@@ -3384,36 +3046,36 @@
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:6" ht="30">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" ht="54" customHeight="1">
+      <c r="A50" s="28"/>
+      <c r="B50" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:6" ht="54" customHeight="1">
-      <c r="A50" s="22"/>
-      <c r="B50" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="E50" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F50" s="15"/>
     </row>
@@ -3435,95 +3097,95 @@
       <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:6" ht="30">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="28"/>
+      <c r="B55" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="E55" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F55" s="15"/>
+    </row>
+    <row r="57" spans="1:6" ht="30">
+      <c r="A57" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F54" s="7"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="22"/>
-      <c r="B55" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D55" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E57" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="F55" s="15"/>
-    </row>
-    <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="22" t="s">
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="28"/>
+      <c r="B58" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="E58" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F58" s="15"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="F57" s="7"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="22"/>
-      <c r="B58" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D58" s="4" t="s">
+      <c r="D60" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F58" s="15"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="22" t="s">
+      <c r="E60" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="28"/>
+      <c r="B61" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="F60" s="7"/>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="22"/>
-      <c r="B61" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>218</v>
-      </c>
       <c r="E61" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F61" s="7"/>
     </row>
@@ -3598,7 +3260,7 @@
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="133" spans="3:3">
@@ -3609,12 +3271,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="A60:A61"/>
     <mergeCell ref="A35:A36"/>
@@ -3623,6 +3279,12 @@
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3630,10 +3292,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408F3E09-3E51-47C3-BF64-60484BEC4CC8}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3649,32 +3312,32 @@
     <row r="1" spans="1:6" ht="18.75">
       <c r="B1" s="3"/>
       <c r="C1" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>220</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>221</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
@@ -3682,7 +3345,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>222</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
@@ -3690,7 +3353,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>223</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3702,117 +3365,119 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="22" t="s">
-        <v>224</v>
+      <c r="A9" s="28" t="s">
+        <v>388</v>
       </c>
       <c r="B9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>227</v>
+        <v>389</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="22"/>
+      <c r="A10" s="28"/>
       <c r="B10" t="s">
-        <v>228</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="15"/>
+        <v>390</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="D11" s="23"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="22" t="s">
-        <v>229</v>
+      <c r="A12" s="28" t="s">
+        <v>391</v>
       </c>
       <c r="B12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="15"/>
+        <v>392</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="22"/>
+      <c r="A13" s="28"/>
       <c r="B13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="15"/>
+        <v>393</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="D14" s="23"/>
-      <c r="E14" s="15"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="22" t="s">
-        <v>233</v>
+      <c r="A15" s="28" t="s">
+        <v>395</v>
       </c>
       <c r="B15" t="s">
-        <v>234</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="D15" s="23"/>
+        <v>396</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="22"/>
+      <c r="A16" s="28"/>
       <c r="B16" t="s">
-        <v>236</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+        <v>397</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="D17" s="23"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="22" t="s">
-        <v>237</v>
+      <c r="A18" s="28" t="s">
+        <v>399</v>
       </c>
       <c r="B18" t="s">
-        <v>238</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="D18" s="23"/>
+        <v>400</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="22"/>
+      <c r="A19" s="28"/>
       <c r="B19" t="s">
-        <v>240</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
+        <v>401</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="18.75">
       <c r="A22" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>242</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30">
@@ -3820,7 +3485,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30">
@@ -3828,7 +3493,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3840,123 +3505,123 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="22" t="s">
-        <v>245</v>
+      <c r="A29" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>246</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>248</v>
+        <v>221</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="22"/>
+      <c r="A30" s="28"/>
       <c r="B30" t="s">
-        <v>249</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
+        <v>224</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="22"/>
+      <c r="A31" s="28"/>
       <c r="B31" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="C31" t="s">
-        <v>251</v>
-      </c>
-      <c r="D31" s="23"/>
+        <v>226</v>
+      </c>
+      <c r="D31" s="26"/>
       <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="D32" s="23"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="15"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="22" t="s">
-        <v>252</v>
+      <c r="A33" s="28" t="s">
+        <v>227</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D33" s="23"/>
+        <v>229</v>
+      </c>
+      <c r="D33" s="26"/>
       <c r="E33" s="15"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="22"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="4" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D34" s="23"/>
+        <v>231</v>
+      </c>
+      <c r="D34" s="26"/>
       <c r="E34" s="15"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="D35" s="23"/>
+      <c r="D35" s="26"/>
       <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5" ht="30">
       <c r="A36" s="5" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D36" s="23"/>
+        <v>234</v>
+      </c>
+      <c r="D36" s="26"/>
       <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="D37" s="23"/>
+      <c r="D37" s="26"/>
       <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="22" t="s">
-        <v>260</v>
+      <c r="A38" s="28" t="s">
+        <v>235</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D38" s="23"/>
+        <v>237</v>
+      </c>
+      <c r="D38" s="26"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="22"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="4" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D39" s="23"/>
+        <v>239</v>
+      </c>
+      <c r="D39" s="26"/>
     </row>
     <row r="42" spans="1:5" ht="18.75">
       <c r="A42" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>266</v>
+        <v>403</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30">
@@ -3964,7 +3629,7 @@
         <v>33</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3972,7 +3637,7 @@
         <v>31</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3984,123 +3649,123 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="22" t="s">
-        <v>269</v>
+      <c r="A49" s="28" t="s">
+        <v>243</v>
       </c>
       <c r="B49" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="C49" t="s">
-        <v>271</v>
-      </c>
-      <c r="D49" s="23" t="s">
-        <v>272</v>
+        <v>245</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="22"/>
+      <c r="A50" s="28"/>
       <c r="B50" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="C50" t="s">
-        <v>274</v>
-      </c>
-      <c r="D50" s="23"/>
+        <v>248</v>
+      </c>
+      <c r="D50" s="26"/>
       <c r="E50" s="15"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="D51" s="23"/>
+      <c r="D51" s="26"/>
       <c r="E51" s="15"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="22" t="s">
-        <v>275</v>
+      <c r="A52" s="28" t="s">
+        <v>249</v>
       </c>
       <c r="B52" t="s">
-        <v>276</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="D52" s="23"/>
+        <v>250</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="D52" s="26"/>
       <c r="E52" s="15"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="22"/>
+      <c r="A53" s="28"/>
       <c r="B53" t="s">
-        <v>278</v>
-      </c>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
+        <v>252</v>
+      </c>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
       <c r="E53" s="15"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="D54" s="23"/>
+      <c r="D54" s="26"/>
       <c r="E54" s="15"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="22" t="s">
-        <v>279</v>
+      <c r="A55" s="28" t="s">
+        <v>253</v>
       </c>
       <c r="B55" t="s">
-        <v>280</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="D55" s="23"/>
+        <v>254</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="D55" s="26"/>
       <c r="E55" s="15"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="22"/>
+      <c r="A56" s="28"/>
       <c r="B56" t="s">
-        <v>282</v>
-      </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+        <v>256</v>
+      </c>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
       <c r="E56" s="15"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="D57" s="23"/>
+      <c r="D57" s="26"/>
       <c r="E57" s="15"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="22" t="s">
-        <v>283</v>
+      <c r="A58" s="28" t="s">
+        <v>257</v>
       </c>
       <c r="B58" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="C58" t="s">
-        <v>285</v>
-      </c>
-      <c r="D58" s="23"/>
+        <v>259</v>
+      </c>
+      <c r="D58" s="26"/>
       <c r="E58" s="15"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="22"/>
+      <c r="A59" s="28"/>
       <c r="B59" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="C59" t="s">
-        <v>287</v>
-      </c>
-      <c r="D59" s="23"/>
+        <v>261</v>
+      </c>
+      <c r="D59" s="26"/>
     </row>
     <row r="62" spans="1:5" ht="18.75">
       <c r="A62" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>289</v>
+        <v>404</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30">
@@ -4108,7 +3773,7 @@
         <v>33</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="30">
@@ -4116,7 +3781,7 @@
         <v>31</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -4128,150 +3793,712 @@
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="22" t="s">
-        <v>292</v>
+      <c r="A69" s="28" t="s">
+        <v>265</v>
       </c>
       <c r="B69" t="s">
-        <v>293</v>
-      </c>
-      <c r="C69" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="D69" s="23" t="s">
-        <v>295</v>
+        <v>266</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="D69" s="26" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="22"/>
+      <c r="A70" s="28"/>
       <c r="B70" t="s">
-        <v>296</v>
-      </c>
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
+        <v>269</v>
+      </c>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23" t="e" vm="5">
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="22" t="s">
-        <v>297</v>
+      <c r="A72" s="28" t="s">
+        <v>270</v>
       </c>
       <c r="B72" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="C72" t="s">
-        <v>299</v>
-      </c>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
+        <v>272</v>
+      </c>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="26"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="22"/>
+      <c r="A73" s="28"/>
       <c r="B73" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
       <c r="C73" t="s">
-        <v>301</v>
-      </c>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
+        <v>274</v>
+      </c>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="22" t="s">
-        <v>302</v>
+      <c r="A75" s="28" t="s">
+        <v>275</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="D75" s="23"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="23"/>
+        <v>277</v>
+      </c>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="22"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="4" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
-      <c r="F76" s="23"/>
+        <v>279</v>
+      </c>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="26"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="D77" s="23"/>
-      <c r="E77" s="23"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="22" t="s">
-        <v>307</v>
+      <c r="A78" s="28" t="s">
+        <v>280</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="D78" s="23"/>
+        <v>282</v>
+      </c>
+      <c r="D78" s="26"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="22"/>
+      <c r="A79" s="28"/>
       <c r="B79" s="4" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="D79" s="23"/>
+        <v>284</v>
+      </c>
+      <c r="D79" s="26"/>
+    </row>
+    <row r="82" spans="1:6" ht="18.75">
+      <c r="A82" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" ht="30">
+      <c r="A84" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="B86" s="3"/>
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="B88" s="3"/>
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B89" t="s">
+        <v>94</v>
+      </c>
+      <c r="C89" t="s">
+        <v>93</v>
+      </c>
+      <c r="D89" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="E89" t="s">
+        <v>93</v>
+      </c>
+      <c r="F89" s="7"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="28"/>
+      <c r="B90" t="s">
+        <v>92</v>
+      </c>
+      <c r="C90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" t="s">
+        <v>91</v>
+      </c>
+      <c r="F90" s="7"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="B91" s="3"/>
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F92" s="7"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="28"/>
+      <c r="B93" t="s">
+        <v>87</v>
+      </c>
+      <c r="C93" s="26"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="26"/>
+      <c r="F93" s="7"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="B94" s="3"/>
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B95" t="s">
+        <v>85</v>
+      </c>
+      <c r="C95" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E95" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F95" s="7"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="28"/>
+      <c r="B96" t="s">
+        <v>82</v>
+      </c>
+      <c r="C96" s="26"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="26"/>
+      <c r="F96" s="7"/>
+    </row>
+    <row r="97" spans="1:6" ht="18.75">
+      <c r="B97" s="3"/>
+      <c r="D97" s="6"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F98" s="7"/>
+    </row>
+    <row r="101" spans="1:6" ht="18.75">
+      <c r="A101" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="30">
+      <c r="A103" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="30">
+      <c r="A104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D106" s="3"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="28" t="s">
+        <v>409</v>
+      </c>
+      <c r="B108" t="s">
+        <v>410</v>
+      </c>
+      <c r="C108" s="26" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="39" customHeight="1">
+      <c r="A109" s="28"/>
+      <c r="B109" t="s">
+        <v>411</v>
+      </c>
+      <c r="C109" s="26"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="28" t="s">
+        <v>413</v>
+      </c>
+      <c r="B111" t="s">
+        <v>414</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="28"/>
+      <c r="B112" t="s">
+        <v>415</v>
+      </c>
+      <c r="C112" s="26"/>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="28" t="s">
+        <v>417</v>
+      </c>
+      <c r="B114" t="s">
+        <v>418</v>
+      </c>
+      <c r="C114" s="26" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="28"/>
+      <c r="B115" t="s">
+        <v>419</v>
+      </c>
+      <c r="C115" s="26"/>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="28" t="s">
+        <v>420</v>
+      </c>
+      <c r="B117" t="s">
+        <v>421</v>
+      </c>
+      <c r="C117" s="26" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="28"/>
+      <c r="B118" t="s">
+        <v>422</v>
+      </c>
+      <c r="C118" s="26"/>
+    </row>
+    <row r="121" spans="1:4" ht="18.75">
+      <c r="A121" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="B125" s="3"/>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="B127" s="3"/>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B128" t="s">
+        <v>71</v>
+      </c>
+      <c r="C128" t="s">
+        <v>70</v>
+      </c>
+      <c r="D128" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="28"/>
+      <c r="B129" t="s">
+        <v>69</v>
+      </c>
+      <c r="C129" t="s">
+        <v>68</v>
+      </c>
+      <c r="D129" s="26"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="B130" s="3"/>
+      <c r="D130" s="26"/>
+    </row>
+    <row r="131" spans="1:4" ht="30">
+      <c r="A131" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D131" s="26"/>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="28"/>
+      <c r="B132" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D132" s="26"/>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="B133" s="3"/>
+      <c r="D133" s="26"/>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D134" s="26"/>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="28"/>
+      <c r="B135" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D135" s="26"/>
+    </row>
+    <row r="138" spans="1:4" ht="18.75">
+      <c r="A138" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D138" s="5"/>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D139" s="4"/>
+    </row>
+    <row r="140" spans="1:4" ht="30">
+      <c r="A140" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D140" s="4"/>
+    </row>
+    <row r="141" spans="1:4" ht="30">
+      <c r="A141" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="B142" s="3"/>
+      <c r="D142" s="5"/>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="B144" s="3"/>
+      <c r="D144" s="3"/>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D145" s="3"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="28"/>
+      <c r="B146" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D146" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="B147" s="3"/>
+      <c r="D147" s="26"/>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D148" s="26"/>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="28"/>
+      <c r="B149" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D149" s="26"/>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="B150" s="3"/>
+      <c r="D150" s="26"/>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D151" s="26"/>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="28"/>
+      <c r="B152" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D152" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="53">
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="D146:D151"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="D128:D135"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="E95:E96"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="F71:F76"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="E71:E77"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D79"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D39"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="D49:D59"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A58:A59"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D19"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="D49:D59"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D39"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="F71:F76"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D69:D79"/>
-    <mergeCell ref="E71:E77"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D98" r:id="rId1" xr:uid="{BF91C729-B873-42CB-9FAC-B65685F2F628}"/>
+    <hyperlink ref="D89" r:id="rId2" xr:uid="{779F719F-C5D3-40E3-A9B2-D8255895AF46}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4279,8 +4506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC519D9-D731-4D86-BB4D-07E97EBA3FC8}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4296,32 +4523,32 @@
     <row r="1" spans="1:6" ht="18.75">
       <c r="B1" s="3"/>
       <c r="C1" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
@@ -4329,7 +4556,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4337,7 +4564,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4350,125 +4577,125 @@
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>319</v>
+        <v>291</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="D10" s="25"/>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="22" t="s">
-        <v>320</v>
+      <c r="A11" s="28" t="s">
+        <v>293</v>
       </c>
       <c r="B11" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="C11" t="s">
-        <v>322</v>
-      </c>
-      <c r="D11" s="25"/>
+        <v>295</v>
+      </c>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="22"/>
+      <c r="A12" s="28"/>
       <c r="B12" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="C12" t="s">
-        <v>324</v>
-      </c>
-      <c r="D12" s="25"/>
+        <v>297</v>
+      </c>
+      <c r="D12" s="29"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="D13" s="25"/>
+      <c r="D13" s="29"/>
     </row>
     <row r="14" spans="1:6" ht="30">
-      <c r="A14" s="22" t="s">
-        <v>325</v>
+      <c r="A14" s="28" t="s">
+        <v>298</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>327</v>
-      </c>
-      <c r="D14" s="25"/>
+        <v>299</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="D14" s="29"/>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="22"/>
+      <c r="A15" s="28"/>
       <c r="B15" t="s">
-        <v>328</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="25"/>
+        <v>301</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="29"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="D16" s="25"/>
+      <c r="D16" s="29"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="22" t="s">
-        <v>329</v>
+      <c r="A17" s="28" t="s">
+        <v>302</v>
       </c>
       <c r="B17" t="s">
-        <v>330</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>331</v>
-      </c>
-      <c r="D17" s="25"/>
+        <v>303</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="D17" s="29"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="22"/>
+      <c r="A18" s="28"/>
       <c r="B18" t="s">
-        <v>332</v>
-      </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="25"/>
+        <v>305</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="D19" s="25"/>
+      <c r="D19" s="29"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="22" t="s">
-        <v>333</v>
+      <c r="A20" s="28" t="s">
+        <v>306</v>
       </c>
       <c r="B20" t="s">
-        <v>334</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>335</v>
+        <v>307</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="22"/>
+      <c r="A21" s="28"/>
       <c r="B21" t="s">
-        <v>336</v>
-      </c>
-      <c r="C21" s="23"/>
+        <v>309</v>
+      </c>
+      <c r="C21" s="26"/>
     </row>
     <row r="24" spans="1:4" ht="18.75">
       <c r="A24" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
@@ -4476,7 +4703,7 @@
         <v>33</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30">
@@ -4484,7 +4711,7 @@
         <v>31</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4497,130 +4724,130 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="20" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="B31" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="C31" t="s">
-        <v>343</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>344</v>
+        <v>316</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="D32" s="23"/>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="22" t="s">
-        <v>345</v>
+      <c r="A33" s="28" t="s">
+        <v>317</v>
       </c>
       <c r="B33" t="s">
-        <v>346</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>347</v>
-      </c>
-      <c r="D33" s="23"/>
+        <v>318</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="22"/>
+      <c r="A34" s="28"/>
       <c r="B34" t="s">
-        <v>348</v>
-      </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
+        <v>320</v>
+      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="15"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="D35" s="23"/>
+      <c r="D35" s="26"/>
       <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="22" t="s">
-        <v>349</v>
+      <c r="A36" s="28" t="s">
+        <v>321</v>
       </c>
       <c r="B36" t="s">
-        <v>346</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>350</v>
-      </c>
-      <c r="D36" s="23"/>
+        <v>318</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="D36" s="26"/>
       <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="22"/>
+      <c r="A37" s="28"/>
       <c r="B37" t="s">
-        <v>351</v>
-      </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
+        <v>323</v>
+      </c>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
       <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="D38" s="23"/>
+      <c r="D38" s="26"/>
       <c r="E38" s="15"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="22" t="s">
-        <v>352</v>
+      <c r="A39" s="28" t="s">
+        <v>324</v>
       </c>
       <c r="B39" t="s">
-        <v>353</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>354</v>
-      </c>
-      <c r="D39" s="23"/>
+        <v>325</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="D39" s="26"/>
       <c r="E39" s="15"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="22"/>
+      <c r="A40" s="28"/>
       <c r="B40" t="s">
-        <v>355</v>
-      </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
+        <v>327</v>
+      </c>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="D41" s="23"/>
+      <c r="D41" s="26"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="22" t="s">
-        <v>356</v>
+      <c r="A42" s="28" t="s">
+        <v>328</v>
       </c>
       <c r="B42" t="s">
-        <v>357</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>358</v>
-      </c>
-      <c r="D42" s="23"/>
+        <v>329</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="D42" s="26"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="22"/>
+      <c r="A43" s="28"/>
       <c r="B43" t="s">
-        <v>359</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
+        <v>331</v>
+      </c>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
     </row>
     <row r="46" spans="1:5" ht="18.75">
       <c r="A46" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30">
@@ -4628,7 +4855,7 @@
         <v>33</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -4636,7 +4863,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -4648,108 +4875,108 @@
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="22" t="s">
-        <v>364</v>
+      <c r="A53" s="28" t="s">
+        <v>336</v>
       </c>
       <c r="B53" t="s">
-        <v>365</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>366</v>
+        <v>337</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>338</v>
       </c>
       <c r="E53" s="7"/>
-      <c r="F53" s="23" t="s">
-        <v>367</v>
+      <c r="F53" s="26" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="34.5" customHeight="1">
-      <c r="A54" s="23"/>
+      <c r="A54" s="26"/>
       <c r="B54" t="s">
-        <v>368</v>
-      </c>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
+        <v>340</v>
+      </c>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
       <c r="E54" s="7"/>
-      <c r="F54" s="23"/>
+      <c r="F54" s="26"/>
     </row>
     <row r="56" spans="1:6" ht="30">
       <c r="A56" s="5" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E56" s="15"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="22" t="s">
-        <v>372</v>
+      <c r="A58" s="28" t="s">
+        <v>344</v>
       </c>
       <c r="B58" t="s">
-        <v>373</v>
-      </c>
-      <c r="C58" s="23" t="s">
-        <v>374</v>
+        <v>345</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>346</v>
       </c>
       <c r="E58" s="15"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="22"/>
+      <c r="A59" s="28"/>
       <c r="B59" t="s">
-        <v>375</v>
-      </c>
-      <c r="C59" s="23"/>
+        <v>347</v>
+      </c>
+      <c r="C59" s="26"/>
       <c r="D59" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E59" s="15"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="22" t="s">
-        <v>376</v>
+      <c r="A61" s="28" t="s">
+        <v>348</v>
       </c>
       <c r="B61" t="s">
-        <v>377</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>378</v>
+        <v>349</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>350</v>
       </c>
       <c r="E61" s="15"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="22"/>
+      <c r="A62" s="28"/>
       <c r="B62" t="s">
-        <v>379</v>
-      </c>
-      <c r="C62" s="23"/>
+        <v>351</v>
+      </c>
+      <c r="C62" s="26"/>
       <c r="D62" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E62" s="15"/>
     </row>
     <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>381</v>
+        <v>353</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30">
@@ -4757,7 +4984,7 @@
         <v>33</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>382</v>
+        <v>354</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30">
@@ -4765,7 +4992,7 @@
         <v>31</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>383</v>
+        <v>355</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4778,111 +5005,115 @@
     </row>
     <row r="72" spans="1:6" ht="45">
       <c r="A72" s="5" t="s">
-        <v>384</v>
+        <v>356</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>385</v>
+        <v>357</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>386</v>
+        <v>358</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>387</v>
+        <v>359</v>
       </c>
       <c r="E72" s="15"/>
       <c r="F72" s="4" t="s">
-        <v>388</v>
+        <v>360</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="20" t="s">
-        <v>389</v>
+        <v>361</v>
       </c>
       <c r="B74" t="s">
-        <v>390</v>
+        <v>362</v>
       </c>
       <c r="C74" t="s">
-        <v>391</v>
+        <v>363</v>
       </c>
       <c r="D74" t="s">
-        <v>392</v>
+        <v>364</v>
       </c>
       <c r="E74" s="15"/>
-      <c r="F74" s="23" t="s">
-        <v>393</v>
+      <c r="F74" s="26" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="E75" s="21"/>
-      <c r="F75" s="23"/>
+      <c r="F75" s="26"/>
     </row>
     <row r="76" spans="1:6" ht="30">
       <c r="A76" s="20" t="s">
-        <v>394</v>
+        <v>366</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>395</v>
+        <v>367</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>396</v>
+        <v>368</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>397</v>
+        <v>369</v>
       </c>
       <c r="E76" s="15"/>
       <c r="F76" s="4" t="s">
-        <v>398</v>
+        <v>429</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="30">
       <c r="A78" s="5" t="s">
-        <v>399</v>
+        <v>370</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>400</v>
+        <v>371</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>401</v>
+        <v>372</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>402</v>
+        <v>373</v>
       </c>
       <c r="E78" s="15"/>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="22" t="s">
-        <v>403</v>
+      <c r="A80" s="28" t="s">
+        <v>374</v>
       </c>
       <c r="B80" t="s">
-        <v>404</v>
-      </c>
-      <c r="C80" s="23" t="s">
-        <v>405</v>
-      </c>
-      <c r="D80" s="23" t="s">
-        <v>406</v>
+        <v>375</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>377</v>
       </c>
       <c r="E80" s="15"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="22"/>
+      <c r="A81" s="28"/>
       <c r="B81" t="s">
-        <v>407</v>
-      </c>
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
+        <v>378</v>
+      </c>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
       <c r="E81" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="D9:D19"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="D80:D81"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="C58:C59"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D31:D43"/>
@@ -4894,16 +5125,12 @@
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="D9:D19"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C17:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>